<commit_message>
Change arragements of widgert in date range selection
</commit_message>
<xml_diff>
--- a/ampl-data-input-excel/33-assign-423/33-assign-423.xlsx
+++ b/ampl-data-input-excel/33-assign-423/33-assign-423.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="17"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="expert" sheetId="1" state="visible" r:id="rId3"/>
@@ -2542,8 +2542,8 @@
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J5" activeCellId="0" sqref="J5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2593,8 +2593,8 @@
         <v>45658</v>
       </c>
       <c r="F2" s="31" t="n">
-        <f aca="false">E2+20</f>
-        <v>45678</v>
+        <f aca="false">misc!E2</f>
+        <v>46391</v>
       </c>
       <c r="G2" s="2" t="b">
         <f aca="false">AND(ISNUMBER(E2), E2&gt;misc!A2)</f>
@@ -2953,7 +2953,7 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>

</xml_diff>